<commit_message>
chap 7 externo paises
</commit_message>
<xml_diff>
--- a/xcolanual.xlsx
+++ b/xcolanual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\Uninorte\Uninorte-docencia\bookdown\intro_eco_col\int_eco_co_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AE670E-ADB7-4C70-B36A-D6CA1A60B6F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0833297F-EA37-40E2-84A6-F6CBB5805D96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="127">
   <si>
     <t>Indicator</t>
   </si>
@@ -372,6 +372,36 @@
   </si>
   <si>
     <t>MACL</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Manufactures</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Pharma</t>
+  </si>
+  <si>
+    <t>FuelM</t>
+  </si>
+  <si>
+    <t>MachineryEq</t>
   </si>
 </sst>
 </file>
@@ -793,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C63639-4019-4BA5-A8BD-D6BF1DB7AA05}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2813,32 +2843,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BX21"/>
+  <dimension ref="A1:BY21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="BB4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="AJ9" sqref="AJ9"/>
+      <selection pane="bottomRight" activeCell="BM14" sqref="BM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="76" width="9.109375" customWidth="1"/>
+    <col min="2" max="3" width="66.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="77" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76">
+    <row r="1" spans="1:77">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
@@ -2846,1478 +2876,1508 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
-    </row>
-    <row r="3" spans="1:76">
+      <c r="K1" s="12"/>
+    </row>
+    <row r="3" spans="1:77">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AE3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AR3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AU3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AW3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AX3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AY3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BA3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BB3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BD3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BD3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BH3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BI3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BI3" s="4" t="s">
+      <c r="BJ3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BJ3" s="4" t="s">
+      <c r="BK3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BK3" s="4" t="s">
+      <c r="BL3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BL3" s="4" t="s">
+      <c r="BM3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BM3" s="4" t="s">
+      <c r="BN3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BN3" s="4" t="s">
+      <c r="BO3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BO3" s="4" t="s">
+      <c r="BP3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BP3" s="4" t="s">
+      <c r="BQ3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BQ3" s="4" t="s">
+      <c r="BR3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BR3" s="4" t="s">
+      <c r="BS3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BS3" s="4" t="s">
+      <c r="BT3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BT3" s="4" t="s">
+      <c r="BU3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BU3" s="4" t="s">
+      <c r="BV3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BV3" s="4" t="s">
+      <c r="BW3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BW3" s="4" t="s">
+      <c r="BX3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BX3" s="9" t="s">
+      <c r="BY3" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:76">
+    <row r="4" spans="1:77">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>307</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>335</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>394</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>463</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>473</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>596</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>657</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>584</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>537</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>511</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>461</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>473</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>465</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>433</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>463</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>446</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>548</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>538</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>507</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>510</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>559</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>607</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>727</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>686</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>808</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>1169</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>1509</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>1465</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>1874</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>2403</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>3010</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>3411</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>3924</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>2916</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>3024</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>3001</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>3462</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>3552</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>5102</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>4642</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>5037</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>5717</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>6721</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>7114</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>6900</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>7116</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>8479</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>10126</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>10587</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>11522</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>10890</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <v>11575</v>
       </c>
-      <c r="BD4">
+      <c r="BE4">
         <v>13043</v>
       </c>
-      <c r="BE4">
+      <c r="BF4">
         <v>12290</v>
       </c>
-      <c r="BF4">
+      <c r="BG4">
         <v>11911</v>
       </c>
-      <c r="BG4">
+      <c r="BH4">
         <v>13080</v>
       </c>
-      <c r="BH4">
+      <c r="BI4">
         <v>16224</v>
       </c>
-      <c r="BI4">
+      <c r="BJ4">
         <v>21190</v>
       </c>
-      <c r="BJ4">
+      <c r="BK4">
         <v>24391</v>
       </c>
-      <c r="BK4">
+      <c r="BL4">
         <v>29991</v>
       </c>
-      <c r="BL4">
+      <c r="BM4">
         <v>37626</v>
       </c>
-      <c r="BM4">
+      <c r="BN4">
         <v>32853</v>
       </c>
-      <c r="BN4">
+      <c r="BO4">
         <v>39713</v>
       </c>
-      <c r="BO4">
+      <c r="BP4">
         <v>56915</v>
       </c>
-      <c r="BP4">
+      <c r="BQ4">
         <v>60125</v>
       </c>
-      <c r="BQ4">
+      <c r="BR4">
         <v>58824</v>
       </c>
-      <c r="BR4">
+      <c r="BS4">
         <v>54857</v>
       </c>
-      <c r="BS4">
+      <c r="BT4">
         <v>35691</v>
       </c>
-      <c r="BT4">
+      <c r="BU4">
         <v>31757</v>
       </c>
-      <c r="BU4">
+      <c r="BV4">
         <v>36897</v>
       </c>
-      <c r="BV4">
+      <c r="BW4">
         <v>41774</v>
       </c>
-      <c r="BW4">
+      <c r="BX4">
         <v>39489</v>
       </c>
-      <c r="BX4" s="10">
+      <c r="BY4" s="10">
         <v>31008</v>
       </c>
     </row>
-    <row r="5" spans="1:76">
+    <row r="5" spans="1:77">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>3020</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>2039</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>2056</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>1978</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>2342</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>2302</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>3633</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>2123</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>2450</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>2426</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>2514</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>2722</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>2726</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>2559</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>3680</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>3695</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>3418</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>4273</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>4004</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>3372</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <v>3106</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <v>2883</v>
       </c>
-      <c r="BF5">
+      <c r="BG5">
         <v>2917</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <v>3003</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <v>3571</v>
       </c>
-      <c r="BI5">
+      <c r="BJ5">
         <v>4599</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <v>4922</v>
       </c>
-      <c r="BK5">
+      <c r="BL5">
         <v>5858</v>
       </c>
-      <c r="BL5">
+      <c r="BM5">
         <v>6693</v>
       </c>
-      <c r="BM5">
+      <c r="BN5">
         <v>5971</v>
       </c>
-      <c r="BN5">
+      <c r="BO5">
         <v>5757</v>
       </c>
-      <c r="BO5">
+      <c r="BP5">
         <v>7059</v>
       </c>
-      <c r="BP5">
+      <c r="BQ5">
         <v>6629</v>
       </c>
-      <c r="BQ5">
+      <c r="BR5">
         <v>6674</v>
       </c>
-      <c r="BR5">
+      <c r="BS5">
         <v>7348</v>
       </c>
-      <c r="BS5">
+      <c r="BT5">
         <v>6935</v>
       </c>
-      <c r="BT5">
+      <c r="BU5">
         <v>6865</v>
       </c>
-      <c r="BU5">
+      <c r="BV5">
         <v>7342</v>
       </c>
-      <c r="BV5">
+      <c r="BW5">
         <v>7297</v>
       </c>
-      <c r="BW5">
+      <c r="BX5">
         <v>7360</v>
       </c>
-      <c r="BX5" s="10"/>
-    </row>
-    <row r="6" spans="1:76">
+      <c r="BY5" s="10"/>
+    </row>
+    <row r="6" spans="1:77">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>2832</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>1858</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>1947</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>1883</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>2161</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>2106</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>3434</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>2099</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>2183</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>2149</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>2222</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>2358</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>2291</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>2137</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>3205</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>3146</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>2843</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>3688</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>3419</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>2796</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>2502</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>2233</v>
       </c>
-      <c r="BF6">
+      <c r="BG6">
         <v>2201</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <v>2278</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <v>2821</v>
       </c>
-      <c r="BI6">
+      <c r="BJ6">
         <v>3636</v>
       </c>
-      <c r="BJ6">
+      <c r="BK6">
         <v>3859</v>
       </c>
-      <c r="BK6">
+      <c r="BL6">
         <v>4577</v>
       </c>
-      <c r="BL6">
+      <c r="BM6">
         <v>5403</v>
       </c>
-      <c r="BM6">
+      <c r="BN6">
         <v>4850</v>
       </c>
-      <c r="BN6">
+      <c r="BO6">
         <v>4447</v>
       </c>
-      <c r="BO6">
+      <c r="BP6">
         <v>5722</v>
       </c>
-      <c r="BP6">
+      <c r="BQ6">
         <v>5251</v>
       </c>
-      <c r="BQ6">
+      <c r="BR6">
         <v>5180</v>
       </c>
-      <c r="BR6">
+      <c r="BS6">
         <v>5819</v>
       </c>
-      <c r="BS6">
+      <c r="BT6">
         <v>5505</v>
       </c>
-      <c r="BT6">
+      <c r="BU6">
         <v>5411</v>
       </c>
-      <c r="BU6">
+      <c r="BV6">
         <v>5858</v>
       </c>
-      <c r="BV6">
+      <c r="BW6">
         <v>5718</v>
       </c>
-      <c r="BW6">
+      <c r="BX6">
         <v>5760</v>
       </c>
-      <c r="BX6" s="10"/>
-    </row>
-    <row r="7" spans="1:76">
+      <c r="BY6" s="10"/>
+    </row>
+    <row r="7" spans="1:77">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>122</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>51</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>229</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>444</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>530</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>593</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>682</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>1519</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>1308</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>1864</v>
       </c>
-      <c r="AT7">
+      <c r="AU7">
         <v>2507</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>2100</v>
       </c>
-      <c r="AV7">
+      <c r="AW7">
         <v>1989</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <v>1916</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>1913</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>2839</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <v>3887</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>3684</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <v>3342</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>4769</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <v>5694</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>4565</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
         <v>4372</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <v>5002</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <v>6386</v>
       </c>
-      <c r="BI7">
+      <c r="BJ7">
         <v>8600</v>
       </c>
-      <c r="BJ7">
+      <c r="BK7">
         <v>9955</v>
       </c>
-      <c r="BK7">
+      <c r="BL7">
         <v>11574</v>
       </c>
-      <c r="BL7">
+      <c r="BM7">
         <v>18047</v>
       </c>
-      <c r="BM7">
+      <c r="BN7">
         <v>16296</v>
       </c>
-      <c r="BN7">
+      <c r="BO7">
         <v>23178</v>
       </c>
-      <c r="BO7">
+      <c r="BP7">
         <v>37148</v>
       </c>
-      <c r="BP7">
+      <c r="BQ7">
         <v>40265</v>
       </c>
-      <c r="BQ7">
+      <c r="BR7">
         <v>39938</v>
       </c>
-      <c r="BR7">
+      <c r="BS7">
         <v>36513</v>
       </c>
-      <c r="BS7">
+      <c r="BT7">
         <v>19291</v>
       </c>
-      <c r="BT7">
+      <c r="BU7">
         <v>15107</v>
       </c>
-      <c r="BU7">
+      <c r="BV7">
         <v>20916</v>
       </c>
-      <c r="BV7">
+      <c r="BW7">
         <v>24710</v>
       </c>
-      <c r="BW7">
+      <c r="BX7">
         <v>22011</v>
       </c>
-      <c r="BX7" s="10"/>
-    </row>
-    <row r="8" spans="1:76">
+      <c r="BY7" s="10"/>
+    </row>
+    <row r="8" spans="1:77">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>2496</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>3623</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <v>3274</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <v>4702</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <v>5636</v>
       </c>
-      <c r="BE8">
+      <c r="BF8">
         <v>4465</v>
       </c>
-      <c r="BF8">
+      <c r="BG8">
         <v>4273</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <v>4869</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <v>6175</v>
       </c>
-      <c r="BI8">
+      <c r="BJ8">
         <v>8316</v>
       </c>
-      <c r="BJ8">
+      <c r="BK8">
         <v>9374</v>
       </c>
-      <c r="BK8">
+      <c r="BL8">
         <v>10872</v>
       </c>
-      <c r="BL8">
+      <c r="BM8">
         <v>17295</v>
       </c>
-      <c r="BM8">
+      <c r="BN8">
         <v>15781</v>
       </c>
-      <c r="BN8">
+      <c r="BO8">
         <v>22564</v>
       </c>
-      <c r="BO8">
+      <c r="BP8">
         <v>36482</v>
       </c>
-      <c r="BP8">
+      <c r="BQ8">
         <v>39612</v>
       </c>
-      <c r="BQ8">
+      <c r="BR8">
         <v>39294</v>
       </c>
-      <c r="BR8">
+      <c r="BS8">
         <v>35982</v>
       </c>
-      <c r="BS8">
+      <c r="BT8">
         <v>18840</v>
       </c>
-      <c r="BT8">
+      <c r="BU8">
         <v>14746</v>
       </c>
-      <c r="BU8">
+      <c r="BV8">
         <v>20446</v>
       </c>
-      <c r="BV8">
+      <c r="BW8">
         <v>24212</v>
       </c>
-      <c r="BW8">
+      <c r="BX8">
         <v>21599</v>
       </c>
-      <c r="BX8" s="10"/>
-    </row>
-    <row r="9" spans="1:76">
+      <c r="BY8" s="10"/>
+    </row>
+    <row r="9" spans="1:77">
       <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <v>775</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>795</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>733</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>533</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>531</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>601</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>745</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>899</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>1207</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <v>1421</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <v>1699</v>
       </c>
-      <c r="AU9">
+      <c r="AV9">
         <v>2409</v>
       </c>
-      <c r="AV9">
+      <c r="AW9">
         <v>2200</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <v>2640</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>2791</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>3493</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <v>3138</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>3517</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <v>3454</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <v>3435</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>4240</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <v>4842</v>
       </c>
-      <c r="BF9">
+      <c r="BG9">
         <v>4496</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <v>4495</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <v>6196</v>
       </c>
-      <c r="BI9">
+      <c r="BJ9">
         <v>7357</v>
       </c>
-      <c r="BJ9">
+      <c r="BK9">
         <v>8678</v>
       </c>
-      <c r="BK9">
+      <c r="BL9">
         <v>11753</v>
       </c>
-      <c r="BL9">
+      <c r="BM9">
         <v>11850</v>
       </c>
-      <c r="BM9">
+      <c r="BN9">
         <v>9016</v>
       </c>
-      <c r="BN9">
+      <c r="BO9">
         <v>8751</v>
       </c>
-      <c r="BO9">
+      <c r="BP9">
         <v>9937</v>
       </c>
-      <c r="BP9">
+      <c r="BQ9">
         <v>9954</v>
       </c>
-      <c r="BQ9">
+      <c r="BR9">
         <v>9936</v>
       </c>
-      <c r="BR9">
+      <c r="BS9">
         <v>9396</v>
       </c>
-      <c r="BS9">
+      <c r="BT9">
         <v>8361</v>
       </c>
-      <c r="BT9">
+      <c r="BU9">
         <v>7526</v>
       </c>
-      <c r="BU9">
+      <c r="BV9">
         <v>7721</v>
       </c>
-      <c r="BV9">
+      <c r="BW9">
         <v>8328</v>
       </c>
-      <c r="BW9">
+      <c r="BX9">
         <v>8292</v>
       </c>
-      <c r="BX9" s="10"/>
-    </row>
-    <row r="10" spans="1:76">
+      <c r="BY9" s="10"/>
+    </row>
+    <row r="10" spans="1:77">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AT10">
+      <c r="AU10">
         <v>172</v>
       </c>
-      <c r="AU10">
+      <c r="AV10">
         <v>177</v>
       </c>
-      <c r="AV10">
+      <c r="AW10">
         <v>142</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <v>112</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <v>140</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <v>210</v>
       </c>
-      <c r="AZ10">
+      <c r="BA10">
         <v>200</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <v>211</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <v>174</v>
       </c>
-      <c r="BC10">
+      <c r="BD10">
         <v>224</v>
       </c>
-      <c r="BD10">
+      <c r="BE10">
         <v>311</v>
       </c>
-      <c r="BE10">
+      <c r="BF10">
         <v>347</v>
       </c>
-      <c r="BF10">
+      <c r="BG10">
         <v>371</v>
       </c>
-      <c r="BG10">
+      <c r="BH10">
         <v>517</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <v>819</v>
       </c>
-      <c r="BI10">
+      <c r="BJ10">
         <v>1037</v>
       </c>
-      <c r="BJ10">
+      <c r="BK10">
         <v>1400</v>
       </c>
-      <c r="BK10">
+      <c r="BL10">
         <v>1941</v>
       </c>
-      <c r="BL10">
+      <c r="BM10">
         <v>1258</v>
       </c>
-      <c r="BM10">
+      <c r="BN10">
         <v>962</v>
       </c>
-      <c r="BN10">
+      <c r="BO10">
         <v>1225</v>
       </c>
-      <c r="BO10">
+      <c r="BP10">
         <v>1084</v>
       </c>
-      <c r="BP10">
+      <c r="BQ10">
         <v>1155</v>
       </c>
-      <c r="BQ10">
+      <c r="BR10">
         <v>854</v>
       </c>
-      <c r="BR10">
+      <c r="BS10">
         <v>780</v>
       </c>
-      <c r="BS10">
+      <c r="BT10">
         <v>522</v>
       </c>
-      <c r="BT10">
+      <c r="BU10">
         <v>409</v>
       </c>
-      <c r="BU10">
+      <c r="BV10">
         <v>492</v>
       </c>
-      <c r="BV10">
+      <c r="BW10">
         <v>735</v>
       </c>
-      <c r="BW10">
+      <c r="BX10">
         <v>689</v>
       </c>
-      <c r="BX10" s="10"/>
-    </row>
-    <row r="11" spans="1:76">
+      <c r="BY10" s="10"/>
+    </row>
+    <row r="11" spans="1:77">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AT11">
+      <c r="AU11">
         <v>229</v>
       </c>
-      <c r="AU11">
+      <c r="AV11">
         <v>336</v>
       </c>
-      <c r="AV11">
+      <c r="AW11">
         <v>377</v>
       </c>
-      <c r="AW11">
+      <c r="AX11">
         <v>424</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <v>536</v>
       </c>
-      <c r="AY11">
+      <c r="AZ11">
         <v>806</v>
       </c>
-      <c r="AZ11">
+      <c r="BA11">
         <v>878</v>
       </c>
-      <c r="BA11">
+      <c r="BB11">
         <v>1075</v>
       </c>
-      <c r="BB11">
+      <c r="BC11">
         <v>1092</v>
       </c>
-      <c r="BC11">
+      <c r="BD11">
         <v>1180</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <v>1333</v>
       </c>
-      <c r="BE11">
+      <c r="BF11">
         <v>1362</v>
       </c>
-      <c r="BF11">
+      <c r="BG11">
         <v>1330</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <v>1219</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <v>1542</v>
       </c>
-      <c r="BI11">
+      <c r="BJ11">
         <v>1786</v>
       </c>
-      <c r="BJ11">
+      <c r="BK11">
         <v>2024</v>
       </c>
-      <c r="BK11">
+      <c r="BL11">
         <v>2413</v>
       </c>
-      <c r="BL11">
+      <c r="BM11">
         <v>2951</v>
       </c>
-      <c r="BM11">
+      <c r="BN11">
         <v>2716</v>
       </c>
-      <c r="BN11">
+      <c r="BO11">
         <v>2847</v>
       </c>
-      <c r="BO11">
+      <c r="BP11">
         <v>3312</v>
       </c>
-      <c r="BP11">
+      <c r="BQ11">
         <v>3429</v>
       </c>
-      <c r="BQ11">
+      <c r="BR11">
         <v>3727</v>
       </c>
-      <c r="BR11">
+      <c r="BS11">
         <v>3688</v>
       </c>
-      <c r="BS11">
+      <c r="BT11">
         <v>3423</v>
       </c>
-      <c r="BT11">
+      <c r="BU11">
         <v>3030</v>
       </c>
-      <c r="BU11">
+      <c r="BV11">
         <v>3053</v>
       </c>
-      <c r="BV11">
+      <c r="BW11">
         <v>3211</v>
       </c>
-      <c r="BW11">
+      <c r="BX11">
         <v>3134</v>
       </c>
-      <c r="BX11" s="10"/>
-    </row>
-    <row r="12" spans="1:76">
+      <c r="BY11" s="10"/>
+    </row>
+    <row r="12" spans="1:77">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BC12">
+      <c r="BD12">
         <v>175</v>
       </c>
-      <c r="BD12">
+      <c r="BE12">
         <v>208</v>
       </c>
-      <c r="BE12">
+      <c r="BF12">
         <v>271</v>
       </c>
-      <c r="BF12">
+      <c r="BG12">
         <v>242</v>
       </c>
-      <c r="BG12">
+      <c r="BH12">
         <v>221</v>
       </c>
-      <c r="BH12">
+      <c r="BI12">
         <v>230</v>
       </c>
-      <c r="BI12">
+      <c r="BJ12">
         <v>264</v>
       </c>
-      <c r="BJ12">
+      <c r="BK12">
         <v>294</v>
       </c>
-      <c r="BK12">
+      <c r="BL12">
         <v>308</v>
       </c>
-      <c r="BL12">
+      <c r="BM12">
         <v>372</v>
       </c>
-      <c r="BM12">
+      <c r="BN12">
         <v>412</v>
       </c>
-      <c r="BN12">
+      <c r="BO12">
         <v>362</v>
       </c>
-      <c r="BO12">
+      <c r="BP12">
         <v>413</v>
       </c>
-      <c r="BP12">
+      <c r="BQ12">
         <v>466</v>
       </c>
-      <c r="BQ12">
+      <c r="BR12">
         <v>501</v>
       </c>
-      <c r="BR12">
+      <c r="BS12">
         <v>530</v>
       </c>
-      <c r="BS12">
+      <c r="BT12">
         <v>509</v>
       </c>
-      <c r="BT12">
+      <c r="BU12">
         <v>431</v>
       </c>
-      <c r="BU12">
+      <c r="BV12">
         <v>357</v>
       </c>
-      <c r="BV12">
+      <c r="BW12">
         <v>358</v>
       </c>
-      <c r="BW12">
+      <c r="BX12">
         <v>367</v>
       </c>
-      <c r="BX12" s="10"/>
-    </row>
-    <row r="13" spans="1:76">
+      <c r="BY12" s="10"/>
+    </row>
+    <row r="13" spans="1:77">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AT13">
+      <c r="AU13">
         <v>85</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>195</v>
       </c>
-      <c r="AV13">
+      <c r="AW13">
         <v>162</v>
       </c>
-      <c r="AW13">
+      <c r="AX13">
         <v>431</v>
       </c>
-      <c r="AX13">
+      <c r="AY13">
         <v>514</v>
       </c>
-      <c r="AY13">
+      <c r="AZ13">
         <v>265</v>
       </c>
-      <c r="AZ13">
+      <c r="BA13">
         <v>290</v>
       </c>
-      <c r="BA13">
+      <c r="BB13">
         <v>438</v>
       </c>
-      <c r="BB13">
+      <c r="BC13">
         <v>427</v>
       </c>
-      <c r="BC13">
+      <c r="BD13">
         <v>307</v>
       </c>
-      <c r="BD13">
+      <c r="BE13">
         <v>562</v>
       </c>
-      <c r="BE13">
+      <c r="BF13">
         <v>828</v>
       </c>
-      <c r="BF13">
+      <c r="BG13">
         <v>663</v>
       </c>
-      <c r="BG13">
+      <c r="BH13">
         <v>430</v>
       </c>
-      <c r="BH13">
+      <c r="BI13">
         <v>911</v>
       </c>
-      <c r="BI13">
+      <c r="BJ13">
         <v>1265</v>
       </c>
-      <c r="BJ13">
+      <c r="BK13">
         <v>1520</v>
       </c>
-      <c r="BK13">
+      <c r="BL13">
         <v>2208</v>
       </c>
-      <c r="BL13">
+      <c r="BM13">
         <v>1884</v>
       </c>
-      <c r="BM13">
+      <c r="BN13">
         <v>1428</v>
       </c>
-      <c r="BN13">
+      <c r="BO13">
         <v>1265</v>
       </c>
-      <c r="BO13">
+      <c r="BP13">
         <v>1721</v>
       </c>
-      <c r="BP13">
+      <c r="BQ13">
         <v>1493</v>
       </c>
-      <c r="BQ13">
+      <c r="BR13">
         <v>1833</v>
       </c>
-      <c r="BR13">
+      <c r="BS13">
         <v>1530</v>
       </c>
-      <c r="BS13">
+      <c r="BT13">
         <v>1424</v>
       </c>
-      <c r="BT13">
+      <c r="BU13">
         <v>1464</v>
       </c>
-      <c r="BU13">
+      <c r="BV13">
         <v>1527</v>
       </c>
-      <c r="BV13">
+      <c r="BW13">
         <v>1571</v>
       </c>
-      <c r="BW13">
+      <c r="BX13">
         <v>1631</v>
       </c>
-      <c r="BX13" s="10"/>
-    </row>
-    <row r="14" spans="1:76">
+      <c r="BY13" s="10"/>
+    </row>
+    <row r="14" spans="1:77">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>5</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>4</v>
-      </c>
-      <c r="AL14">
-        <v>2</v>
       </c>
       <c r="AM14">
         <v>2</v>
@@ -4326,10 +4386,10 @@
         <v>2</v>
       </c>
       <c r="AO14">
+        <v>2</v>
+      </c>
+      <c r="AP14">
         <v>1</v>
-      </c>
-      <c r="AP14">
-        <v>2</v>
       </c>
       <c r="AQ14">
         <v>2</v>
@@ -4344,280 +4404,283 @@
         <v>2</v>
       </c>
       <c r="AU14">
+        <v>2</v>
+      </c>
+      <c r="AV14">
         <v>5</v>
       </c>
-      <c r="AV14">
+      <c r="AW14">
         <v>4</v>
       </c>
-      <c r="AW14">
+      <c r="AX14">
         <v>14</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>12</v>
-      </c>
-      <c r="AY14">
-        <v>6</v>
       </c>
       <c r="AZ14">
         <v>6</v>
       </c>
       <c r="BA14">
+        <v>6</v>
+      </c>
+      <c r="BB14">
         <v>4</v>
       </c>
-      <c r="BB14">
+      <c r="BC14">
         <v>5</v>
       </c>
-      <c r="BC14">
+      <c r="BD14">
         <v>7</v>
       </c>
-      <c r="BD14">
+      <c r="BE14">
         <v>12</v>
       </c>
-      <c r="BE14">
+      <c r="BF14">
         <v>15</v>
       </c>
-      <c r="BF14">
+      <c r="BG14">
         <v>23</v>
       </c>
-      <c r="BG14">
+      <c r="BH14">
         <v>25</v>
       </c>
-      <c r="BH14">
+      <c r="BI14">
         <v>56</v>
       </c>
-      <c r="BI14">
+      <c r="BJ14">
         <v>57</v>
       </c>
-      <c r="BJ14">
+      <c r="BK14">
         <v>59</v>
       </c>
-      <c r="BK14">
+      <c r="BL14">
         <v>41</v>
       </c>
-      <c r="BL14">
+      <c r="BM14">
         <v>54</v>
       </c>
-      <c r="BM14">
+      <c r="BN14">
         <v>76</v>
       </c>
-      <c r="BN14">
+      <c r="BO14">
         <v>58</v>
       </c>
-      <c r="BO14">
+      <c r="BP14">
         <v>56</v>
       </c>
-      <c r="BP14">
+      <c r="BQ14">
         <v>75</v>
       </c>
-      <c r="BQ14">
+      <c r="BR14">
         <v>92</v>
       </c>
-      <c r="BR14">
+      <c r="BS14">
         <v>97</v>
-      </c>
-      <c r="BS14">
-        <v>89</v>
       </c>
       <c r="BT14">
         <v>89</v>
       </c>
       <c r="BU14">
+        <v>89</v>
+      </c>
+      <c r="BV14">
         <v>102</v>
       </c>
-      <c r="BV14">
+      <c r="BW14">
         <v>99</v>
       </c>
-      <c r="BW14">
+      <c r="BX14">
         <v>114</v>
       </c>
-      <c r="BX14" s="10"/>
-    </row>
-    <row r="15" spans="1:76">
+      <c r="BY14" s="10"/>
+    </row>
+    <row r="15" spans="1:77">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AY15">
+      <c r="AZ15">
         <v>2</v>
       </c>
-      <c r="AZ15">
+      <c r="BA15">
         <v>3</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>1</v>
       </c>
-      <c r="BB15">
+      <c r="BC15">
         <v>3</v>
       </c>
-      <c r="BC15">
+      <c r="BD15">
         <v>2</v>
       </c>
-      <c r="BD15">
+      <c r="BE15">
         <v>3</v>
-      </c>
-      <c r="BE15">
-        <v>8</v>
       </c>
       <c r="BF15">
         <v>8</v>
       </c>
       <c r="BG15">
+        <v>8</v>
+      </c>
+      <c r="BH15">
         <v>6</v>
       </c>
-      <c r="BH15">
+      <c r="BI15">
         <v>25</v>
       </c>
-      <c r="BI15">
+      <c r="BJ15">
         <v>10</v>
       </c>
-      <c r="BJ15">
+      <c r="BK15">
         <v>13</v>
       </c>
-      <c r="BK15">
+      <c r="BL15">
         <v>14</v>
       </c>
-      <c r="BL15">
+      <c r="BM15">
         <v>16</v>
       </c>
-      <c r="BM15">
+      <c r="BN15">
         <v>12</v>
       </c>
-      <c r="BN15">
+      <c r="BO15">
         <v>11</v>
       </c>
-      <c r="BO15">
+      <c r="BP15">
         <v>9</v>
       </c>
-      <c r="BP15">
+      <c r="BQ15">
         <v>10</v>
       </c>
-      <c r="BQ15">
+      <c r="BR15">
         <v>19</v>
       </c>
-      <c r="BR15">
+      <c r="BS15">
         <v>20</v>
       </c>
-      <c r="BS15">
+      <c r="BT15">
         <v>16</v>
       </c>
-      <c r="BT15">
+      <c r="BU15">
         <v>17</v>
       </c>
-      <c r="BU15">
+      <c r="BV15">
         <v>31</v>
       </c>
-      <c r="BV15">
+      <c r="BW15">
         <v>37</v>
       </c>
-      <c r="BW15">
+      <c r="BX15">
         <v>24</v>
       </c>
-      <c r="BX15" s="10"/>
-    </row>
-    <row r="16" spans="1:76">
+      <c r="BY15" s="10"/>
+    </row>
+    <row r="16" spans="1:77">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AY16">
+      <c r="AZ16">
         <v>5</v>
       </c>
-      <c r="AZ16">
+      <c r="BA16">
         <v>3</v>
-      </c>
-      <c r="BA16">
-        <v>2</v>
       </c>
       <c r="BB16">
         <v>2</v>
       </c>
       <c r="BC16">
+        <v>2</v>
+      </c>
+      <c r="BD16">
         <v>5</v>
       </c>
-      <c r="BD16">
+      <c r="BE16">
         <v>8</v>
       </c>
-      <c r="BE16">
+      <c r="BF16">
         <v>7</v>
       </c>
-      <c r="BF16">
+      <c r="BG16">
         <v>15</v>
       </c>
-      <c r="BG16">
+      <c r="BH16">
         <v>19</v>
       </c>
-      <c r="BH16">
+      <c r="BI16">
         <v>30</v>
       </c>
-      <c r="BI16">
+      <c r="BJ16">
         <v>46</v>
       </c>
-      <c r="BJ16">
+      <c r="BK16">
         <v>41</v>
       </c>
-      <c r="BK16">
+      <c r="BL16">
         <v>27</v>
       </c>
-      <c r="BL16">
+      <c r="BM16">
         <v>35</v>
       </c>
-      <c r="BM16">
+      <c r="BN16">
         <v>60</v>
       </c>
-      <c r="BN16">
+      <c r="BO16">
         <v>45</v>
       </c>
-      <c r="BO16">
+      <c r="BP16">
         <v>43</v>
       </c>
-      <c r="BP16">
+      <c r="BQ16">
         <v>59</v>
       </c>
-      <c r="BQ16">
+      <c r="BR16">
         <v>63</v>
       </c>
-      <c r="BR16">
+      <c r="BS16">
         <v>59</v>
       </c>
-      <c r="BS16">
+      <c r="BT16">
         <v>48</v>
       </c>
-      <c r="BT16">
+      <c r="BU16">
         <v>43</v>
       </c>
-      <c r="BU16">
+      <c r="BV16">
         <v>40</v>
       </c>
-      <c r="BV16">
+      <c r="BW16">
         <v>33</v>
       </c>
-      <c r="BW16">
+      <c r="BX16">
         <v>28</v>
       </c>
-      <c r="BX16" s="10"/>
-    </row>
-    <row r="17" spans="1:76">
+      <c r="BY16" s="10"/>
+    </row>
+    <row r="17" spans="1:77">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="AY17">
-        <v>0</v>
       </c>
       <c r="AZ17">
         <v>0</v>
@@ -4626,10 +4689,10 @@
         <v>0</v>
       </c>
       <c r="BB17">
+        <v>0</v>
+      </c>
+      <c r="BC17">
         <v>1</v>
-      </c>
-      <c r="BC17">
-        <v>0</v>
       </c>
       <c r="BD17">
         <v>0</v>
@@ -4647,369 +4710,375 @@
         <v>0</v>
       </c>
       <c r="BI17">
+        <v>0</v>
+      </c>
+      <c r="BJ17">
         <v>1</v>
       </c>
-      <c r="BJ17">
+      <c r="BK17">
         <v>5</v>
       </c>
-      <c r="BK17">
+      <c r="BL17">
         <v>1</v>
       </c>
-      <c r="BL17">
+      <c r="BM17">
         <v>3</v>
       </c>
-      <c r="BM17">
+      <c r="BN17">
         <v>4</v>
       </c>
-      <c r="BN17">
+      <c r="BO17">
         <v>3</v>
       </c>
-      <c r="BO17">
+      <c r="BP17">
         <v>4</v>
       </c>
-      <c r="BP17">
+      <c r="BQ17">
         <v>6</v>
       </c>
-      <c r="BQ17">
+      <c r="BR17">
         <v>10</v>
       </c>
-      <c r="BR17">
+      <c r="BS17">
         <v>17</v>
       </c>
-      <c r="BS17">
+      <c r="BT17">
         <v>25</v>
       </c>
-      <c r="BT17">
+      <c r="BU17">
         <v>29</v>
       </c>
-      <c r="BU17">
+      <c r="BV17">
         <v>32</v>
       </c>
-      <c r="BV17">
+      <c r="BW17">
         <v>29</v>
       </c>
-      <c r="BW17">
+      <c r="BX17">
         <v>63</v>
       </c>
-      <c r="BX17" s="10"/>
-    </row>
-    <row r="18" spans="1:76">
+      <c r="BY17" s="10"/>
+    </row>
+    <row r="18" spans="1:77">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BD18">
+      <c r="BE18">
         <v>289</v>
       </c>
-      <c r="BE18">
+      <c r="BF18">
         <v>488</v>
       </c>
-      <c r="BF18">
+      <c r="BG18">
         <v>374</v>
       </c>
-      <c r="BG18">
+      <c r="BH18">
         <v>173</v>
       </c>
-      <c r="BH18">
+      <c r="BI18">
         <v>471</v>
       </c>
-      <c r="BI18">
+      <c r="BJ18">
         <v>746</v>
       </c>
-      <c r="BJ18">
+      <c r="BK18">
         <v>876</v>
       </c>
-      <c r="BK18">
+      <c r="BL18">
         <v>1307</v>
       </c>
-      <c r="BL18">
+      <c r="BM18">
         <v>766</v>
       </c>
-      <c r="BM18">
+      <c r="BN18">
         <v>397</v>
       </c>
-      <c r="BN18">
+      <c r="BO18">
         <v>587</v>
       </c>
-      <c r="BO18">
+      <c r="BP18">
         <v>965</v>
       </c>
-      <c r="BP18">
+      <c r="BQ18">
         <v>610</v>
       </c>
-      <c r="BQ18">
+      <c r="BR18">
         <v>914</v>
       </c>
-      <c r="BR18">
+      <c r="BS18">
         <v>606</v>
       </c>
-      <c r="BS18">
+      <c r="BT18">
         <v>576</v>
       </c>
-      <c r="BT18">
+      <c r="BU18">
         <v>624</v>
       </c>
-      <c r="BU18">
+      <c r="BV18">
         <v>634</v>
       </c>
-      <c r="BV18">
+      <c r="BW18">
         <v>716</v>
       </c>
-      <c r="BW18">
+      <c r="BX18">
         <v>764</v>
       </c>
-      <c r="BX18" s="10"/>
-    </row>
-    <row r="19" spans="1:76">
+      <c r="BY18" s="10"/>
+    </row>
+    <row r="19" spans="1:77">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AT19">
+      <c r="AU19">
         <v>6</v>
       </c>
-      <c r="AU19">
+      <c r="AV19">
         <v>20</v>
       </c>
-      <c r="AV19">
+      <c r="AW19">
         <v>19</v>
       </c>
-      <c r="AW19">
+      <c r="AX19">
         <v>48</v>
       </c>
-      <c r="AX19">
+      <c r="AY19">
         <v>52</v>
       </c>
-      <c r="AY19">
+      <c r="AZ19">
         <v>83</v>
       </c>
-      <c r="AZ19">
+      <c r="BA19">
         <v>108</v>
       </c>
-      <c r="BA19">
+      <c r="BB19">
         <v>193</v>
       </c>
-      <c r="BB19">
+      <c r="BC19">
         <v>160</v>
       </c>
-      <c r="BC19">
+      <c r="BD19">
         <v>75</v>
       </c>
-      <c r="BD19">
+      <c r="BE19">
         <v>226</v>
       </c>
-      <c r="BE19">
+      <c r="BF19">
         <v>433</v>
       </c>
-      <c r="BF19">
+      <c r="BG19">
         <v>338</v>
       </c>
-      <c r="BG19">
+      <c r="BH19">
         <v>117</v>
       </c>
-      <c r="BH19">
+      <c r="BI19">
         <v>413</v>
       </c>
-      <c r="BI19">
+      <c r="BJ19">
         <v>647</v>
       </c>
-      <c r="BJ19">
+      <c r="BK19">
         <v>744</v>
       </c>
-      <c r="BK19">
+      <c r="BL19">
         <v>1130</v>
       </c>
-      <c r="BL19">
+      <c r="BM19">
         <v>533</v>
       </c>
-      <c r="BM19">
+      <c r="BN19">
         <v>248</v>
       </c>
-      <c r="BN19">
+      <c r="BO19">
         <v>341</v>
       </c>
-      <c r="BO19">
+      <c r="BP19">
         <v>393</v>
       </c>
-      <c r="BP19">
+      <c r="BQ19">
         <v>563</v>
       </c>
-      <c r="BQ19">
+      <c r="BR19">
         <v>839</v>
       </c>
-      <c r="BR19">
+      <c r="BS19">
         <v>524</v>
       </c>
-      <c r="BS19">
+      <c r="BT19">
         <v>483</v>
       </c>
-      <c r="BT19">
+      <c r="BU19">
         <v>538</v>
       </c>
-      <c r="BU19">
+      <c r="BV19">
         <v>523</v>
       </c>
-      <c r="BV19">
+      <c r="BW19">
         <v>632</v>
       </c>
-      <c r="BW19">
+      <c r="BX19">
         <v>638</v>
       </c>
-      <c r="BX19" s="10"/>
-    </row>
-    <row r="20" spans="1:76">
+      <c r="BY19" s="10"/>
+    </row>
+    <row r="20" spans="1:77">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AJ20">
+      <c r="AK20">
         <v>135</v>
       </c>
-      <c r="AK20">
+      <c r="AL20">
         <v>108</v>
       </c>
-      <c r="AL20">
+      <c r="AM20">
         <v>87</v>
       </c>
-      <c r="AM20">
+      <c r="AN20">
         <v>67</v>
       </c>
-      <c r="AN20">
+      <c r="AO20">
         <v>73</v>
       </c>
-      <c r="AO20">
+      <c r="AP20">
         <v>72</v>
       </c>
-      <c r="AP20">
+      <c r="AQ20">
         <v>87</v>
       </c>
-      <c r="AQ20">
+      <c r="AR20">
         <v>109</v>
       </c>
-      <c r="AR20">
+      <c r="AS20">
         <v>96</v>
       </c>
-      <c r="AS20">
+      <c r="AT20">
         <v>116</v>
       </c>
-      <c r="AT20">
+      <c r="AU20">
         <v>133</v>
       </c>
-      <c r="AU20">
+      <c r="AV20">
         <v>173</v>
       </c>
-      <c r="AV20">
+      <c r="AW20">
         <v>177</v>
       </c>
-      <c r="AW20">
+      <c r="AX20">
         <v>203</v>
       </c>
-      <c r="AX20">
+      <c r="AY20">
         <v>212</v>
       </c>
-      <c r="AY20">
+      <c r="AZ20">
         <v>278</v>
       </c>
-      <c r="AZ20">
+      <c r="BA20">
         <v>279</v>
       </c>
-      <c r="BA20">
+      <c r="BB20">
         <v>294</v>
       </c>
-      <c r="BB20">
+      <c r="BC20">
         <v>267</v>
       </c>
-      <c r="BC20">
+      <c r="BD20">
         <v>238</v>
       </c>
-      <c r="BD20">
+      <c r="BE20">
         <v>268</v>
       </c>
-      <c r="BE20">
+      <c r="BF20">
         <v>264</v>
       </c>
-      <c r="BF20">
+      <c r="BG20">
         <v>205</v>
       </c>
-      <c r="BG20">
+      <c r="BH20">
         <v>228</v>
       </c>
-      <c r="BH20">
+      <c r="BI20">
         <v>320</v>
       </c>
-      <c r="BI20">
+      <c r="BJ20">
         <v>356</v>
       </c>
-      <c r="BJ20">
+      <c r="BK20">
         <v>383</v>
       </c>
-      <c r="BK20">
+      <c r="BL20">
         <v>628</v>
       </c>
-      <c r="BL20">
+      <c r="BM20">
         <v>858</v>
       </c>
-      <c r="BM20">
+      <c r="BN20">
         <v>639</v>
       </c>
-      <c r="BN20">
+      <c r="BO20">
         <v>414</v>
       </c>
-      <c r="BO20">
+      <c r="BP20">
         <v>486</v>
       </c>
-      <c r="BP20">
+      <c r="BQ20">
         <v>454</v>
       </c>
-      <c r="BQ20">
+      <c r="BR20">
         <v>386</v>
       </c>
-      <c r="BR20">
+      <c r="BS20">
         <v>361</v>
       </c>
-      <c r="BS20">
+      <c r="BT20">
         <v>314</v>
       </c>
-      <c r="BT20">
+      <c r="BU20">
         <v>277</v>
       </c>
-      <c r="BU20">
+      <c r="BV20">
         <v>280</v>
       </c>
-      <c r="BV20">
+      <c r="BW20">
         <v>287</v>
       </c>
-      <c r="BW20">
+      <c r="BX20">
         <v>278</v>
       </c>
-      <c r="BX20" s="10"/>
-    </row>
-    <row r="21" spans="1:76">
+      <c r="BY20" s="10"/>
+    </row>
+    <row r="21" spans="1:77">
       <c r="A21" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -5041,131 +5110,132 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
-      <c r="AJ21" s="3">
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3">
         <v>119</v>
       </c>
-      <c r="AK21" s="3">
+      <c r="AL21" s="3">
         <v>118</v>
       </c>
-      <c r="AL21" s="3">
+      <c r="AM21" s="3">
         <v>135</v>
       </c>
-      <c r="AM21" s="3">
+      <c r="AN21" s="3">
         <v>62</v>
       </c>
-      <c r="AN21" s="3">
+      <c r="AO21" s="3">
         <v>43</v>
       </c>
-      <c r="AO21" s="3">
+      <c r="AP21" s="3">
         <v>55</v>
       </c>
-      <c r="AP21" s="3">
+      <c r="AQ21" s="3">
         <v>84</v>
       </c>
-      <c r="AQ21" s="3">
+      <c r="AR21" s="3">
         <v>112</v>
       </c>
-      <c r="AR21" s="3">
+      <c r="AS21" s="3">
         <v>209</v>
       </c>
-      <c r="AS21" s="3">
+      <c r="AT21" s="3">
         <v>331</v>
       </c>
-      <c r="AT21" s="3">
+      <c r="AU21" s="3">
         <v>460</v>
       </c>
-      <c r="AU21" s="3">
+      <c r="AV21" s="3">
         <v>593</v>
       </c>
-      <c r="AV21" s="3">
+      <c r="AW21" s="3">
         <v>446</v>
       </c>
-      <c r="AW21" s="3">
+      <c r="AX21" s="3">
         <v>534</v>
       </c>
-      <c r="AX21" s="3">
+      <c r="AY21" s="3">
         <v>523</v>
       </c>
-      <c r="AY21" s="3">
+      <c r="AZ21" s="3">
         <v>552</v>
       </c>
-      <c r="AZ21" s="3">
+      <c r="BA21" s="3">
         <v>476</v>
       </c>
-      <c r="BA21" s="3">
+      <c r="BB21" s="3">
         <v>445</v>
       </c>
-      <c r="BB21" s="3">
+      <c r="BC21" s="3">
         <v>433</v>
       </c>
-      <c r="BC21" s="3">
+      <c r="BD21" s="3">
         <v>427</v>
       </c>
-      <c r="BD21" s="3">
+      <c r="BE21" s="3">
         <v>520</v>
       </c>
-      <c r="BE21" s="3">
+      <c r="BF21" s="3">
         <v>572</v>
       </c>
-      <c r="BF21" s="3">
+      <c r="BG21" s="3">
         <v>523</v>
       </c>
-      <c r="BG21" s="3">
+      <c r="BH21" s="3">
         <v>637</v>
       </c>
-      <c r="BH21" s="3">
+      <c r="BI21" s="3">
         <v>868</v>
       </c>
-      <c r="BI21" s="3">
+      <c r="BJ21" s="3">
         <v>908</v>
       </c>
-      <c r="BJ21" s="3">
+      <c r="BK21" s="3">
         <v>962</v>
       </c>
-      <c r="BK21" s="3">
+      <c r="BL21" s="3">
         <v>1351</v>
       </c>
-      <c r="BL21" s="3">
+      <c r="BM21" s="3">
         <v>1222</v>
       </c>
-      <c r="BM21" s="3">
+      <c r="BN21" s="3">
         <v>592</v>
-      </c>
-      <c r="BN21" s="3">
-        <v>650</v>
       </c>
       <c r="BO21" s="3">
         <v>650</v>
       </c>
       <c r="BP21" s="3">
+        <v>650</v>
+      </c>
+      <c r="BQ21" s="3">
         <v>703</v>
       </c>
-      <c r="BQ21" s="3">
+      <c r="BR21" s="3">
         <v>615</v>
       </c>
-      <c r="BR21" s="3">
+      <c r="BS21" s="3">
         <v>546</v>
       </c>
-      <c r="BS21" s="3">
+      <c r="BT21" s="3">
         <v>518</v>
       </c>
-      <c r="BT21" s="3">
+      <c r="BU21" s="3">
         <v>425</v>
       </c>
-      <c r="BU21" s="3">
+      <c r="BV21" s="3">
         <v>426</v>
-      </c>
-      <c r="BV21" s="3">
-        <v>467</v>
       </c>
       <c r="BW21" s="3">
         <v>467</v>
       </c>
-      <c r="BX21" s="5"/>
+      <c r="BX21" s="3">
+        <v>467</v>
+      </c>
+      <c r="BY21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>